<commit_message>
completed readme. final commit
</commit_message>
<xml_diff>
--- a/Output Data.xlsx
+++ b/Output Data.xlsx
@@ -733,6 +733,84 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38381517935258092"/>
+                  <c:y val="-5.8814158646835812E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>output!$B$2:$B$13</c:f>
@@ -833,13 +911,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="558999936"/>
-        <c:axId val="559002680"/>
+        <c:axId val="577169104"/>
+        <c:axId val="577168712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="558999936"/>
+        <c:axId val="577169104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="22"/>
+          <c:min val="8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -936,12 +1016,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559002680"/>
+        <c:crossAx val="577168712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="559002680"/>
+        <c:axId val="577168712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="558999936"/>
+        <c:crossAx val="577169104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1960,7 +2040,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>